<commit_message>
Employee module add,Business partner check address validation
</commit_message>
<xml_diff>
--- a/Troy.Web/Troy.Web/App_Data/ExcelFiles/BPartner.xlsx
+++ b/Troy.Web/Troy.Web/App_Data/ExcelFiles/BPartner.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>BusinessPartner Name</t>
   </si>
@@ -144,25 +144,22 @@
     <t>madurai</t>
   </si>
   <si>
-    <t>TestGroup</t>
-  </si>
-  <si>
     <t>Test type</t>
   </si>
   <si>
-    <t>Test Price List</t>
-  </si>
-  <si>
-    <t>TroyPlus</t>
-  </si>
-  <si>
-    <t>Kamarajar Salai</t>
-  </si>
-  <si>
-    <t>B/S</t>
-  </si>
-  <si>
     <t>testBPtestbulk</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>KKThoppu</t>
+  </si>
+  <si>
+    <t>Sales</t>
   </si>
 </sst>
 </file>
@@ -507,7 +504,7 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -627,13 +624,13 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Businesspartner,employee bulk addition validations
</commit_message>
<xml_diff>
--- a/Troy.Web/Troy.Web/App_Data/ExcelFiles/BPartner.xlsx
+++ b/Troy.Web/Troy.Web/App_Data/ExcelFiles/BPartner.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>BusinessPartner Name</t>
   </si>
@@ -117,12 +117,6 @@
     <t>india</t>
   </si>
   <si>
-    <t>tn</t>
-  </si>
-  <si>
-    <t>mdu</t>
-  </si>
-  <si>
     <t>aaa@troy-plus.co.in</t>
   </si>
   <si>
@@ -144,12 +138,6 @@
     <t>madurai</t>
   </si>
   <si>
-    <t>Test type</t>
-  </si>
-  <si>
-    <t>testBPtestbulk</t>
-  </si>
-  <si>
     <t>Camera</t>
   </si>
   <si>
@@ -160,6 +148,21 @@
   </si>
   <si>
     <t>Sales</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>test fax</t>
+  </si>
+  <si>
+    <t>master id check</t>
+  </si>
+  <si>
+    <t>web camera</t>
+  </si>
+  <si>
+    <t>sales</t>
   </si>
 </sst>
 </file>
@@ -501,9 +504,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
@@ -516,15 +519,16 @@
     <col min="10" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:33">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -598,125 +602,131 @@
         <v>23</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
         <v>32</v>
       </c>
       <c r="J2">
-        <v>625004</v>
+        <v>625144</v>
       </c>
       <c r="K2" t="s">
         <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
         <v>32</v>
       </c>
       <c r="Q2">
-        <v>625885</v>
+        <v>625020</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="T2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2">
+        <v>2653333</v>
+      </c>
+      <c r="W2">
+        <v>2598888</v>
+      </c>
+      <c r="X2">
+        <v>9955869555</v>
+      </c>
+      <c r="Y2" t="s">
         <v>45</v>
       </c>
-      <c r="U2" t="s">
-        <v>46</v>
-      </c>
-      <c r="V2">
-        <v>144</v>
-      </c>
-      <c r="W2">
-        <v>111</v>
-      </c>
-      <c r="X2">
-        <v>111</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB2" t="s">
         <v>35</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AC2" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AD2" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2">
-        <v>100000</v>
-      </c>
-      <c r="AF2" s="1">
+      <c r="AE2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2">
+        <v>250000</v>
+      </c>
+      <c r="AG2" s="1">
         <v>41907</v>
       </c>
     </row>

</xml_diff>